<commit_message>
Modificando el menu de configuraciones
</commit_message>
<xml_diff>
--- a/storage/app/utils/Statuses.xlsx
+++ b/storage/app/utils/Statuses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crm.atalaya\storage\app\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CB5491-1A34-42BE-8072-AD738B4D946E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6370325C-3F20-49BC-8B1F-FCFFDB7D2547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Estado</t>
   </si>
@@ -135,9 +135,6 @@
     <t>in_setting</t>
   </si>
   <si>
-    <t>default-lead-status</t>
-  </si>
-  <si>
     <t>9c27e649-574a-47eb-82af-851c5d425434</t>
   </si>
   <si>
@@ -174,10 +171,28 @@
     <t>#f9c851</t>
   </si>
   <si>
-    <t>default-manage-lead-status</t>
-  </si>
-  <si>
     <t>default-client-status</t>
+  </si>
+  <si>
+    <t>En Gestión</t>
+  </si>
+  <si>
+    <t>Cuando el cliente</t>
+  </si>
+  <si>
+    <t>#328ae2</t>
+  </si>
+  <si>
+    <t>asignation-lead-status[lead]</t>
+  </si>
+  <si>
+    <t>asignation-lead-status[manage]</t>
+  </si>
+  <si>
+    <t>default-lead-status|revertion-lead-status[lead]</t>
+  </si>
+  <si>
+    <t>default-manage-lead-status|revertion-lead-status[manage]</t>
   </si>
 </sst>
 </file>
@@ -511,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +539,7 @@
     <col min="3" max="3" width="60.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -565,7 +580,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -585,7 +600,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -593,16 +608,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -610,13 +628,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>34</v>
@@ -627,13 +645,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>34</v>
@@ -644,16 +662,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -661,13 +679,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -678,13 +696,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>11</v>
@@ -695,13 +713,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
@@ -712,19 +730,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>49</v>
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -732,16 +747,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,16 +767,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -766,16 +787,33 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
+      <c r="E15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>